<commit_message>
-Placed now-unused code in "trashcode" folder. -Added persistent modchip settings initialization, fetch and write on flash memory. -Added function to program flash memory without rebooting. -Added few new settings in persistent settings struct. -Configurable timout delay on IconMenu. Taken from persistent settings. -Removed annoying warnings when compiling main code and imagebld tool. -Few other small things. It's a new project so lot of code change happens at once!
</commit_message>
<xml_diff>
--- a/saveMemoryMap.xlsx
+++ b/saveMemoryMap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>LCD</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>reserved2</t>
+  </si>
+  <si>
+    <t>NB_lines</t>
+  </si>
+  <si>
+    <t>lines_length</t>
+  </si>
+  <si>
+    <t>boot_timeout</t>
   </si>
 </sst>
 </file>
@@ -189,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -202,6 +211,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -508,8 +523,8 @@
   <dimension ref="A1:D257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97:A257"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +559,7 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -552,131 +567,135 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -685,10 +704,10 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -697,8 +716,8 @@
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -707,8 +726,8 @@
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -717,1788 +736,1790 @@
       <c r="B20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="B21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="B22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D77" s="3"/>
+      <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>96</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D97" s="3"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>97</v>
       </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>98</v>
       </c>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>99</v>
       </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>100</v>
       </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>101</v>
       </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>102</v>
       </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>103</v>
       </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>104</v>
       </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>105</v>
       </c>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>106</v>
       </c>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>107</v>
       </c>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>108</v>
       </c>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>109</v>
       </c>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>110</v>
       </c>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>111</v>
       </c>
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>112</v>
       </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>113</v>
       </c>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>114</v>
       </c>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>115</v>
       </c>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>116</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B117" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>117</v>
       </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>118</v>
       </c>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>119</v>
       </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>120</v>
       </c>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>121</v>
       </c>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>122</v>
       </c>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>123</v>
       </c>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>124</v>
       </c>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>125</v>
       </c>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>126</v>
       </c>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>127</v>
       </c>
-      <c r="B128" s="3"/>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>128</v>
       </c>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="6"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>129</v>
       </c>
-      <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>130</v>
       </c>
-      <c r="B131" s="3"/>
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>131</v>
       </c>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>132</v>
       </c>
-      <c r="B133" s="3"/>
-      <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>133</v>
       </c>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
-      <c r="D134" s="3"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>134</v>
       </c>
-      <c r="B135" s="3"/>
-      <c r="C135" s="3"/>
-      <c r="D135" s="3"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>135</v>
       </c>
-      <c r="B136" s="3"/>
-      <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>136</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B137" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C137" s="3"/>
-      <c r="D137" s="3"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>137</v>
       </c>
-      <c r="B138" s="3"/>
-      <c r="C138" s="3"/>
-      <c r="D138" s="3"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>138</v>
       </c>
-      <c r="B139" s="3"/>
-      <c r="C139" s="3"/>
-      <c r="D139" s="3"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>139</v>
       </c>
-      <c r="B140" s="3"/>
-      <c r="C140" s="3"/>
-      <c r="D140" s="3"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>140</v>
       </c>
-      <c r="B141" s="3"/>
-      <c r="C141" s="3"/>
-      <c r="D141" s="3"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>141</v>
       </c>
-      <c r="B142" s="3"/>
-      <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>142</v>
       </c>
-      <c r="B143" s="3"/>
-      <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>143</v>
       </c>
-      <c r="B144" s="3"/>
-      <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>144</v>
       </c>
-      <c r="B145" s="3"/>
-      <c r="C145" s="3"/>
-      <c r="D145" s="3"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>145</v>
       </c>
-      <c r="B146" s="3"/>
-      <c r="C146" s="3"/>
-      <c r="D146" s="3"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>146</v>
       </c>
-      <c r="B147" s="3"/>
-      <c r="C147" s="3"/>
-      <c r="D147" s="3"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>147</v>
       </c>
-      <c r="B148" s="3"/>
-      <c r="C148" s="3"/>
-      <c r="D148" s="3"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>148</v>
       </c>
-      <c r="B149" s="3"/>
-      <c r="C149" s="3"/>
-      <c r="D149" s="3"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>149</v>
       </c>
-      <c r="B150" s="3"/>
-      <c r="C150" s="3"/>
-      <c r="D150" s="3"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>150</v>
       </c>
-      <c r="B151" s="3"/>
-      <c r="C151" s="3"/>
-      <c r="D151" s="3"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>151</v>
       </c>
-      <c r="B152" s="3"/>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>152</v>
       </c>
-      <c r="B153" s="3"/>
-      <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>153</v>
       </c>
-      <c r="B154" s="3"/>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>154</v>
       </c>
-      <c r="B155" s="3"/>
-      <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>155</v>
       </c>
-      <c r="B156" s="3"/>
-      <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>156</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B157" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>157</v>
       </c>
-      <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>158</v>
       </c>
-      <c r="B159" s="3"/>
-      <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>159</v>
       </c>
-      <c r="B160" s="3"/>
-      <c r="C160" s="3"/>
-      <c r="D160" s="3"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>160</v>
       </c>
-      <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>161</v>
       </c>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>162</v>
       </c>
-      <c r="B163" s="3"/>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>163</v>
       </c>
-      <c r="B164" s="3"/>
-      <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>164</v>
       </c>
-      <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-      <c r="D165" s="3"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>165</v>
       </c>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="3"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>166</v>
       </c>
-      <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
-      <c r="D167" s="3"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>167</v>
       </c>
-      <c r="B168" s="3"/>
-      <c r="C168" s="3"/>
-      <c r="D168" s="3"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>168</v>
       </c>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
-      <c r="D169" s="3"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>169</v>
       </c>
-      <c r="B170" s="3"/>
-      <c r="C170" s="3"/>
-      <c r="D170" s="3"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>170</v>
       </c>
-      <c r="B171" s="3"/>
-      <c r="C171" s="3"/>
-      <c r="D171" s="3"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>171</v>
       </c>
-      <c r="B172" s="3"/>
-      <c r="C172" s="3"/>
-      <c r="D172" s="3"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>172</v>
       </c>
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
-      <c r="D173" s="3"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>173</v>
       </c>
-      <c r="B174" s="3"/>
-      <c r="C174" s="3"/>
-      <c r="D174" s="3"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>174</v>
       </c>
-      <c r="B175" s="3"/>
-      <c r="C175" s="3"/>
-      <c r="D175" s="3"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>175</v>
       </c>
-      <c r="B176" s="3"/>
-      <c r="C176" s="3"/>
-      <c r="D176" s="3"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>176</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="B177" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C177" s="3"/>
-      <c r="D177" s="3"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>177</v>
       </c>
-      <c r="B178" s="3"/>
-      <c r="C178" s="3"/>
-      <c r="D178" s="3"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>178</v>
       </c>
-      <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
-      <c r="D179" s="3"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>179</v>
       </c>
-      <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
-      <c r="D180" s="3"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>180</v>
       </c>
-      <c r="B181" s="3"/>
-      <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>181</v>
       </c>
-      <c r="B182" s="3"/>
-      <c r="C182" s="3"/>
-      <c r="D182" s="3"/>
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
+      <c r="D182" s="6"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>182</v>
       </c>
-      <c r="B183" s="3"/>
-      <c r="C183" s="3"/>
-      <c r="D183" s="3"/>
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>183</v>
       </c>
-      <c r="B184" s="3"/>
-      <c r="C184" s="3"/>
-      <c r="D184" s="3"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
+      <c r="D184" s="6"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>184</v>
       </c>
-      <c r="B185" s="3"/>
-      <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="6"/>
+      <c r="D185" s="6"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>185</v>
       </c>
-      <c r="B186" s="3"/>
-      <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>186</v>
       </c>
-      <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
+      <c r="B187" s="6"/>
+      <c r="C187" s="6"/>
+      <c r="D187" s="6"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>187</v>
       </c>
-      <c r="B188" s="3"/>
-      <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
+      <c r="B188" s="6"/>
+      <c r="C188" s="6"/>
+      <c r="D188" s="6"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>188</v>
       </c>
-      <c r="B189" s="3"/>
-      <c r="C189" s="3"/>
-      <c r="D189" s="3"/>
+      <c r="B189" s="6"/>
+      <c r="C189" s="6"/>
+      <c r="D189" s="6"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>189</v>
       </c>
-      <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
+      <c r="B190" s="6"/>
+      <c r="C190" s="6"/>
+      <c r="D190" s="6"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>190</v>
       </c>
-      <c r="B191" s="3"/>
-      <c r="C191" s="3"/>
-      <c r="D191" s="3"/>
+      <c r="B191" s="6"/>
+      <c r="C191" s="6"/>
+      <c r="D191" s="6"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>191</v>
       </c>
-      <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
+      <c r="B192" s="6"/>
+      <c r="C192" s="6"/>
+      <c r="D192" s="6"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>192</v>
       </c>
-      <c r="B193" s="3"/>
-      <c r="C193" s="3"/>
-      <c r="D193" s="3"/>
+      <c r="B193" s="6"/>
+      <c r="C193" s="6"/>
+      <c r="D193" s="6"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>193</v>
       </c>
-      <c r="B194" s="3"/>
-      <c r="C194" s="3"/>
-      <c r="D194" s="3"/>
+      <c r="B194" s="6"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>194</v>
       </c>
-      <c r="B195" s="3"/>
-      <c r="C195" s="3"/>
-      <c r="D195" s="3"/>
+      <c r="B195" s="6"/>
+      <c r="C195" s="6"/>
+      <c r="D195" s="6"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>195</v>
       </c>
-      <c r="B196" s="3"/>
-      <c r="C196" s="3"/>
-      <c r="D196" s="3"/>
+      <c r="B196" s="6"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="6"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>196</v>
       </c>
-      <c r="B197" s="3" t="s">
+      <c r="B197" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="6"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>197</v>
       </c>
-      <c r="B198" s="3"/>
-      <c r="C198" s="3"/>
-      <c r="D198" s="3"/>
+      <c r="B198" s="6"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="6"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>198</v>
       </c>
-      <c r="B199" s="3"/>
-      <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
+      <c r="B199" s="6"/>
+      <c r="C199" s="6"/>
+      <c r="D199" s="6"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>199</v>
       </c>
-      <c r="B200" s="3"/>
-      <c r="C200" s="3"/>
-      <c r="D200" s="3"/>
+      <c r="B200" s="6"/>
+      <c r="C200" s="6"/>
+      <c r="D200" s="6"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>200</v>
       </c>
-      <c r="B201" s="3"/>
-      <c r="C201" s="3"/>
-      <c r="D201" s="3"/>
+      <c r="B201" s="6"/>
+      <c r="C201" s="6"/>
+      <c r="D201" s="6"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>201</v>
       </c>
-      <c r="B202" s="3"/>
-      <c r="C202" s="3"/>
-      <c r="D202" s="3"/>
+      <c r="B202" s="6"/>
+      <c r="C202" s="6"/>
+      <c r="D202" s="6"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>202</v>
       </c>
-      <c r="B203" s="3"/>
-      <c r="C203" s="3"/>
-      <c r="D203" s="3"/>
+      <c r="B203" s="6"/>
+      <c r="C203" s="6"/>
+      <c r="D203" s="6"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>203</v>
       </c>
-      <c r="B204" s="3"/>
-      <c r="C204" s="3"/>
-      <c r="D204" s="3"/>
+      <c r="B204" s="6"/>
+      <c r="C204" s="6"/>
+      <c r="D204" s="6"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>204</v>
       </c>
-      <c r="B205" s="3"/>
-      <c r="C205" s="3"/>
-      <c r="D205" s="3"/>
+      <c r="B205" s="6"/>
+      <c r="C205" s="6"/>
+      <c r="D205" s="6"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>205</v>
       </c>
-      <c r="B206" s="3"/>
-      <c r="C206" s="3"/>
-      <c r="D206" s="3"/>
+      <c r="B206" s="6"/>
+      <c r="C206" s="6"/>
+      <c r="D206" s="6"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>206</v>
       </c>
-      <c r="B207" s="3"/>
-      <c r="C207" s="3"/>
-      <c r="D207" s="3"/>
+      <c r="B207" s="6"/>
+      <c r="C207" s="6"/>
+      <c r="D207" s="6"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>207</v>
       </c>
-      <c r="B208" s="3"/>
-      <c r="C208" s="3"/>
-      <c r="D208" s="3"/>
+      <c r="B208" s="6"/>
+      <c r="C208" s="6"/>
+      <c r="D208" s="6"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>208</v>
       </c>
-      <c r="B209" s="3"/>
-      <c r="C209" s="3"/>
-      <c r="D209" s="3"/>
+      <c r="B209" s="6"/>
+      <c r="C209" s="6"/>
+      <c r="D209" s="6"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>209</v>
       </c>
-      <c r="B210" s="3"/>
-      <c r="C210" s="3"/>
-      <c r="D210" s="3"/>
+      <c r="B210" s="6"/>
+      <c r="C210" s="6"/>
+      <c r="D210" s="6"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>210</v>
       </c>
-      <c r="B211" s="3"/>
-      <c r="C211" s="3"/>
-      <c r="D211" s="3"/>
+      <c r="B211" s="6"/>
+      <c r="C211" s="6"/>
+      <c r="D211" s="6"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>211</v>
       </c>
-      <c r="B212" s="3"/>
-      <c r="C212" s="3"/>
-      <c r="D212" s="3"/>
+      <c r="B212" s="6"/>
+      <c r="C212" s="6"/>
+      <c r="D212" s="6"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>212</v>
       </c>
-      <c r="B213" s="3"/>
-      <c r="C213" s="3"/>
-      <c r="D213" s="3"/>
+      <c r="B213" s="6"/>
+      <c r="C213" s="6"/>
+      <c r="D213" s="6"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>213</v>
       </c>
-      <c r="B214" s="3"/>
-      <c r="C214" s="3"/>
-      <c r="D214" s="3"/>
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>214</v>
       </c>
-      <c r="B215" s="3"/>
-      <c r="C215" s="3"/>
-      <c r="D215" s="3"/>
+      <c r="B215" s="6"/>
+      <c r="C215" s="6"/>
+      <c r="D215" s="6"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>215</v>
       </c>
-      <c r="B216" s="3"/>
-      <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
+      <c r="B216" s="6"/>
+      <c r="C216" s="6"/>
+      <c r="D216" s="6"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>216</v>
       </c>
-      <c r="B217" s="3"/>
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
+      <c r="D217" s="6"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>217</v>
       </c>
-      <c r="B218" s="3"/>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3"/>
+      <c r="B218" s="6"/>
+      <c r="C218" s="6"/>
+      <c r="D218" s="6"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>218</v>
       </c>
-      <c r="B219" s="3"/>
-      <c r="C219" s="3"/>
-      <c r="D219" s="3"/>
+      <c r="B219" s="6"/>
+      <c r="C219" s="6"/>
+      <c r="D219" s="6"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>219</v>
       </c>
-      <c r="B220" s="3"/>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3"/>
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
+      <c r="D220" s="6"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>220</v>
       </c>
-      <c r="B221" s="3"/>
-      <c r="C221" s="3"/>
-      <c r="D221" s="3"/>
+      <c r="B221" s="6"/>
+      <c r="C221" s="6"/>
+      <c r="D221" s="6"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>221</v>
       </c>
-      <c r="B222" s="3"/>
-      <c r="C222" s="3"/>
-      <c r="D222" s="3"/>
+      <c r="B222" s="6"/>
+      <c r="C222" s="6"/>
+      <c r="D222" s="6"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>222</v>
       </c>
-      <c r="B223" s="3"/>
-      <c r="C223" s="3"/>
-      <c r="D223" s="3"/>
+      <c r="B223" s="6"/>
+      <c r="C223" s="6"/>
+      <c r="D223" s="6"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>223</v>
       </c>
-      <c r="B224" s="3"/>
-      <c r="C224" s="3"/>
-      <c r="D224" s="3"/>
+      <c r="B224" s="6"/>
+      <c r="C224" s="6"/>
+      <c r="D224" s="6"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>224</v>
       </c>
-      <c r="B225" s="3"/>
-      <c r="C225" s="3"/>
-      <c r="D225" s="3"/>
+      <c r="B225" s="6"/>
+      <c r="C225" s="6"/>
+      <c r="D225" s="6"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>225</v>
       </c>
-      <c r="B226" s="3"/>
-      <c r="C226" s="3"/>
-      <c r="D226" s="3"/>
+      <c r="B226" s="6"/>
+      <c r="C226" s="6"/>
+      <c r="D226" s="6"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>226</v>
       </c>
-      <c r="B227" s="3"/>
-      <c r="C227" s="3"/>
-      <c r="D227" s="3"/>
+      <c r="B227" s="6"/>
+      <c r="C227" s="6"/>
+      <c r="D227" s="6"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>227</v>
       </c>
-      <c r="B228" s="3"/>
-      <c r="C228" s="3"/>
-      <c r="D228" s="3"/>
+      <c r="B228" s="6"/>
+      <c r="C228" s="6"/>
+      <c r="D228" s="6"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>228</v>
       </c>
-      <c r="B229" s="3"/>
-      <c r="C229" s="3"/>
-      <c r="D229" s="3"/>
+      <c r="B229" s="6"/>
+      <c r="C229" s="6"/>
+      <c r="D229" s="6"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>229</v>
       </c>
-      <c r="B230" s="3"/>
-      <c r="C230" s="3"/>
-      <c r="D230" s="3"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="6"/>
+      <c r="D230" s="6"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>230</v>
       </c>
-      <c r="B231" s="3"/>
-      <c r="C231" s="3"/>
-      <c r="D231" s="3"/>
+      <c r="B231" s="6"/>
+      <c r="C231" s="6"/>
+      <c r="D231" s="6"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>231</v>
       </c>
-      <c r="B232" s="3"/>
-      <c r="C232" s="3"/>
-      <c r="D232" s="3"/>
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
+      <c r="D232" s="6"/>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>232</v>
       </c>
-      <c r="B233" s="3"/>
-      <c r="C233" s="3"/>
-      <c r="D233" s="3"/>
+      <c r="B233" s="6"/>
+      <c r="C233" s="6"/>
+      <c r="D233" s="6"/>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>233</v>
       </c>
-      <c r="B234" s="3"/>
-      <c r="C234" s="3"/>
-      <c r="D234" s="3"/>
+      <c r="B234" s="6"/>
+      <c r="C234" s="6"/>
+      <c r="D234" s="6"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
         <v>234</v>
       </c>
-      <c r="B235" s="3"/>
-      <c r="C235" s="3"/>
-      <c r="D235" s="3"/>
+      <c r="B235" s="6"/>
+      <c r="C235" s="6"/>
+      <c r="D235" s="6"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>235</v>
       </c>
-      <c r="B236" s="3"/>
-      <c r="C236" s="3"/>
-      <c r="D236" s="3"/>
+      <c r="B236" s="6"/>
+      <c r="C236" s="6"/>
+      <c r="D236" s="6"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>236</v>
       </c>
-      <c r="B237" s="3"/>
-      <c r="C237" s="3"/>
-      <c r="D237" s="3"/>
+      <c r="B237" s="6"/>
+      <c r="C237" s="6"/>
+      <c r="D237" s="6"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>237</v>
       </c>
-      <c r="B238" s="3"/>
-      <c r="C238" s="3"/>
-      <c r="D238" s="3"/>
+      <c r="B238" s="6"/>
+      <c r="C238" s="6"/>
+      <c r="D238" s="6"/>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>238</v>
       </c>
-      <c r="B239" s="3"/>
-      <c r="C239" s="3"/>
-      <c r="D239" s="3"/>
+      <c r="B239" s="6"/>
+      <c r="C239" s="6"/>
+      <c r="D239" s="6"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
@@ -2507,8 +2528,8 @@
       <c r="B240" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C240" s="3"/>
-      <c r="D240" s="3"/>
+      <c r="C240" s="6"/>
+      <c r="D240" s="6"/>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
@@ -2517,155 +2538,148 @@
       <c r="B241" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C241" s="3"/>
-      <c r="D241" s="3"/>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>241</v>
       </c>
-      <c r="B242" s="3" t="s">
+      <c r="B242" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C242" s="3"/>
-      <c r="D242" s="3"/>
+      <c r="C242" s="6"/>
+      <c r="D242" s="6"/>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
         <v>242</v>
       </c>
-      <c r="B243" s="3"/>
-      <c r="C243" s="3"/>
-      <c r="D243" s="3"/>
+      <c r="B243" s="6"/>
+      <c r="C243" s="6"/>
+      <c r="D243" s="6"/>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
         <v>243</v>
       </c>
-      <c r="B244" s="3"/>
-      <c r="C244" s="3"/>
-      <c r="D244" s="3"/>
+      <c r="B244" s="6"/>
+      <c r="C244" s="6"/>
+      <c r="D244" s="6"/>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
         <v>244</v>
       </c>
-      <c r="B245" s="3"/>
-      <c r="C245" s="3"/>
-      <c r="D245" s="3"/>
+      <c r="B245" s="6"/>
+      <c r="C245" s="6"/>
+      <c r="D245" s="6"/>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
         <v>245</v>
       </c>
-      <c r="B246" s="3" t="s">
+      <c r="B246" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C246" s="3"/>
-      <c r="D246" s="3"/>
+      <c r="C246" s="6"/>
+      <c r="D246" s="6"/>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
         <v>246</v>
       </c>
-      <c r="B247" s="3"/>
-      <c r="C247" s="3"/>
-      <c r="D247" s="3"/>
+      <c r="B247" s="6"/>
+      <c r="C247" s="6"/>
+      <c r="D247" s="6"/>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
         <v>247</v>
       </c>
-      <c r="B248" s="3"/>
-      <c r="C248" s="3"/>
-      <c r="D248" s="3"/>
+      <c r="B248" s="6"/>
+      <c r="C248" s="6"/>
+      <c r="D248" s="6"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
         <v>248</v>
       </c>
-      <c r="B249" s="3"/>
-      <c r="C249" s="3"/>
-      <c r="D249" s="3"/>
+      <c r="B249" s="6"/>
+      <c r="C249" s="6"/>
+      <c r="D249" s="6"/>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
         <v>249</v>
       </c>
-      <c r="B250" s="3" t="s">
+      <c r="B250" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C250" s="3"/>
-      <c r="D250" s="3"/>
+      <c r="C250" s="6"/>
+      <c r="D250" s="6"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
         <v>250</v>
       </c>
-      <c r="B251" s="3"/>
-      <c r="C251" s="3"/>
-      <c r="D251" s="3"/>
+      <c r="B251" s="6"/>
+      <c r="C251" s="6"/>
+      <c r="D251" s="6"/>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
         <v>251</v>
       </c>
-      <c r="B252" s="3"/>
-      <c r="C252" s="3"/>
-      <c r="D252" s="3"/>
+      <c r="B252" s="6"/>
+      <c r="C252" s="6"/>
+      <c r="D252" s="6"/>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
         <v>252</v>
       </c>
-      <c r="B253" s="3"/>
-      <c r="C253" s="3"/>
-      <c r="D253" s="3"/>
+      <c r="B253" s="6"/>
+      <c r="C253" s="6"/>
+      <c r="D253" s="6"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
         <v>253</v>
       </c>
-      <c r="B254" s="3" t="s">
+      <c r="B254" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C254" s="3"/>
-      <c r="D254" s="3"/>
+      <c r="C254" s="6"/>
+      <c r="D254" s="6"/>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>254</v>
       </c>
-      <c r="B255" s="3"/>
-      <c r="C255" s="3"/>
-      <c r="D255" s="3"/>
+      <c r="B255" s="6"/>
+      <c r="C255" s="6"/>
+      <c r="D255" s="6"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
         <v>255</v>
       </c>
-      <c r="B256" s="3"/>
-      <c r="C256" s="3"/>
-      <c r="D256" s="3"/>
+      <c r="B256" s="6"/>
+      <c r="C256" s="6"/>
+      <c r="D256" s="6"/>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
         <v>256</v>
       </c>
-      <c r="B257" s="3"/>
-      <c r="C257" s="3"/>
-      <c r="D257" s="3"/>
+      <c r="B257" s="6"/>
+      <c r="C257" s="6"/>
+      <c r="D257" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B21:B36"/>
-    <mergeCell ref="B197:B239"/>
-    <mergeCell ref="C97:C257"/>
-    <mergeCell ref="B157:B176"/>
-    <mergeCell ref="B177:B196"/>
-    <mergeCell ref="B254:B257"/>
-    <mergeCell ref="B250:B253"/>
-    <mergeCell ref="B246:B249"/>
+    <mergeCell ref="B22:B36"/>
     <mergeCell ref="B242:B245"/>
     <mergeCell ref="B57:B76"/>
     <mergeCell ref="B77:B96"/>
@@ -2678,8 +2692,15 @@
     <mergeCell ref="C37:C56"/>
     <mergeCell ref="C57:C76"/>
     <mergeCell ref="C77:C96"/>
-    <mergeCell ref="C10:C16"/>
     <mergeCell ref="B37:B56"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B197:B239"/>
+    <mergeCell ref="C97:C257"/>
+    <mergeCell ref="B157:B176"/>
+    <mergeCell ref="B177:B196"/>
+    <mergeCell ref="B254:B257"/>
+    <mergeCell ref="B250:B253"/>
+    <mergeCell ref="B246:B249"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-Changed TABs to 4 spaces in all source files. -Refined checks to detect XBlast chip. Should be usable(limited) on other modchips and in XBE form. -Memory Tester should produce something(will need testing) -Added new persistent setting(altBank) for alternative boot bank. Will be implemented later.
</commit_message>
<xml_diff>
--- a/saveMemoryMap.xlsx
+++ b/saveMemoryMap.xlsx
@@ -1,179 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
+  <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Feuil1"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Feuil2"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Feuil3"</definedName>
+  </definedNames>
+  <calcPr calcMode="auto" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <webPublishing allowPng="1" css="0" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5" count="5">
   <si>
-    <t>byte</t>
-  </si>
-  <si>
-    <t>OS_settings</t>
-  </si>
-  <si>
-    <t>LCD</t>
-  </si>
-  <si>
-    <t>EEProm</t>
+    <t>migrate?</t>
   </si>
   <si>
     <t>migrate?</t>
   </si>
   <si>
-    <t>Backup</t>
-  </si>
-  <si>
     <t>reserved</t>
-  </si>
-  <si>
-    <t>EN_5V?</t>
-  </si>
-  <si>
-    <t>LCD_type</t>
-  </si>
-  <si>
-    <t>NB_lines</t>
-  </si>
-  <si>
-    <t>lines_length</t>
-  </si>
-  <si>
-    <t>Backlight</t>
-  </si>
-  <si>
-    <t>Contrast</t>
-  </si>
-  <si>
-    <t>Display msg. Boot?</t>
-  </si>
-  <si>
-    <t>Custom text?</t>
-  </si>
-  <si>
-    <t>Disp booting BIOS name?</t>
-  </si>
-  <si>
-    <t>Active bank</t>
-  </si>
-  <si>
-    <t>String0</t>
-  </si>
-  <si>
-    <t>Quickboot?</t>
   </si>
   <si>
     <t>selected_item</t>
   </si>
   <si>
-    <t>fan_speed</t>
-  </si>
-  <si>
-    <t>boot_timeout</t>
-  </si>
-  <si>
-    <t>LEDColor</t>
-  </si>
-  <si>
     <t>reserved1</t>
-  </si>
-  <si>
-    <t>BIOS_name0</t>
-  </si>
-  <si>
-    <t>string1</t>
-  </si>
-  <si>
-    <t>BIOS_name1</t>
-  </si>
-  <si>
-    <t>string2</t>
-  </si>
-  <si>
-    <t>Reserved_bank2</t>
-  </si>
-  <si>
-    <t>string3</t>
-  </si>
-  <si>
-    <t>Reserved_bank3</t>
-  </si>
-  <si>
-    <t>Reserved_bank4</t>
-  </si>
-  <si>
-    <t>Reserved_bank5</t>
-  </si>
-  <si>
-    <t>Reserved_bank6</t>
-  </si>
-  <si>
-    <t>Reserved_bank7</t>
-  </si>
-  <si>
-    <t>reserved2</t>
-  </si>
-  <si>
-    <t>Enable Network?</t>
-  </si>
-  <si>
-    <t>Use DHCP?</t>
-  </si>
-  <si>
-    <t>IP address</t>
-  </si>
-  <si>
-    <t>Gateway</t>
-  </si>
-  <si>
-    <t>DNS1</t>
-  </si>
-  <si>
-    <t>DNS2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <b val="0"/>
+      <i val="0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <strike val="0"/>
     </font>
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -185,2258 +73,2261 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+    <border diagonalUp="0" diagonalDown="0">
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FFC7C7C7"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+    <border diagonalUp="0" diagonalDown="0">
+      <left style="none">
+        <color rgb="FFC7C7C7"/>
+      </left>
+      <right style="none">
+        <color rgb="FFC7C7C7"/>
+      </right>
+      <top style="none">
+        <color rgb="FFC7C7C7"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
+    <border diagonalUp="0" diagonalDown="0">
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+    <border diagonalUp="0" diagonalDown="0">
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FFC7C7C7"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf/>
+  </cellStyleXfs>
+  <cellXfs count="9">
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-  </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
     <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D257"/>
+  <dimension ref="A1:AMK257"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.5748987854251"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5748987854251"/>
+    <col min="1" max="1" style="1" width="11.4251" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="1" width="24.5749" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" style="1" width="23.4251" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" style="1" width="11.4251" bestFit="1" customWidth="1"/>
+    <col min="5" max="1025" style="2" width="10.5749" bestFit="1" customWidth="1"/>
+    <col min="1026" max="16384" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1025">
+      <c r="A1" s="3" t="str">
+        <v>byte</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>OS_settings</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>LCD</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>EEProm</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1025">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D2" s="4" t="str">
+        <v>Backup</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1025">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="str">
+        <v>EN_5V?</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:1025">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="str">
+        <v>LCD_type</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:1025">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="str">
+        <v>NB_lines</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:1025">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="str">
+        <v>lines_length</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:1025">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="str">
+        <v>Backlight</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:1025">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="str">
+        <v>Contrast</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:1025">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="str">
+        <v>Display msg. Boot?</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:1025">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="str">
+        <v>Custom text?</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:1025">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>10</v>
-      </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
+      <c r="C11" s="4" t="str">
+        <v>Disp booting BIOS name?</v>
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+    <row r="12" spans="1:1025">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+    <row r="13" spans="1:1025">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+    <row r="14" spans="1:1025">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+    <row r="15" spans="1:1025">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+    <row r="16" spans="1:1025">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+    <row r="17" spans="1:1025">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="4" t="str">
+        <v>Active bank</v>
+      </c>
+      <c r="C17" s="4" t="str">
+        <v>String0</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:1025">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>18</v>
+      <c r="B18" s="5" t="str">
+        <v>Alternate bank</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+    <row r="19" spans="1:1025">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>19</v>
+      <c r="B19" s="4" t="str">
+        <v>Quickboot?</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+    <row r="20" spans="1:1025">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>20</v>
+      <c r="B20" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+    <row r="21" spans="1:1025">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>21</v>
+      <c r="B21" s="6" t="str">
+        <v>fan_speed</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+    <row r="22" spans="1:1025">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>22</v>
+      <c r="B22" s="6" t="str">
+        <v>boot_timeout</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+    <row r="23" spans="1:1025">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>23</v>
+      <c r="B23" s="4" t="str">
+        <v>LEDColor</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+    <row r="24" spans="1:1025">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="str">
+        <v>TSOP Control</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+    <row r="25" spans="1:1025">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+    <row r="26" spans="1:1025">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+    <row r="27" spans="1:1025">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+    <row r="28" spans="1:1025">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+    <row r="29" spans="1:1025">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+    <row r="30" spans="1:1025">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+    <row r="31" spans="1:1025">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
+    <row r="32" spans="1:1025">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
+    <row r="33" spans="1:1025">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
+    <row r="34" spans="1:1025">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="n">
+    <row r="35" spans="1:1025">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="n">
+    <row r="36" spans="1:1025">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
+    <row r="37" spans="1:1025">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>25</v>
+      <c r="B37" s="4" t="str">
+        <v>BIOS_name0</v>
+      </c>
+      <c r="C37" s="4" t="str">
+        <v>string1</v>
       </c>
       <c r="D37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="n">
+    <row r="38" spans="1:1025">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="n">
+    <row r="39" spans="1:1025">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="n">
+    <row r="40" spans="1:1025">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="n">
+    <row r="41" spans="1:1025">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="n">
+    <row r="42" spans="1:1025">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="n">
+    <row r="43" spans="1:1025">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="n">
+    <row r="44" spans="1:1025">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="n">
+    <row r="45" spans="1:1025">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="n">
+    <row r="46" spans="1:1025">
+      <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="n">
+    <row r="47" spans="1:1025">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="n">
+    <row r="48" spans="1:1025">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="n">
+    <row r="49" spans="1:1025">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="n">
+    <row r="50" spans="1:1025">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="n">
+    <row r="51" spans="1:1025">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="n">
+    <row r="52" spans="1:1025">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="n">
+    <row r="53" spans="1:1025">
+      <c r="A53" s="4">
         <v>52</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="n">
+    <row r="54" spans="1:1025">
+      <c r="A54" s="4">
         <v>53</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="n">
+    <row r="55" spans="1:1025">
+      <c r="A55" s="4">
         <v>54</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="n">
+    <row r="56" spans="1:1025">
+      <c r="A56" s="4">
         <v>55</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3" t="n">
+    <row r="57" spans="1:1025">
+      <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>27</v>
+      <c r="B57" s="4" t="str">
+        <v>BIOS_name1</v>
+      </c>
+      <c r="C57" s="4" t="str">
+        <v>string2</v>
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3" t="n">
+    <row r="58" spans="1:1025">
+      <c r="A58" s="4">
         <v>57</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="n">
+    <row r="59" spans="1:1025">
+      <c r="A59" s="4">
         <v>58</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="n">
+    <row r="60" spans="1:1025">
+      <c r="A60" s="4">
         <v>59</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="n">
+    <row r="61" spans="1:1025">
+      <c r="A61" s="4">
         <v>60</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3" t="n">
+    <row r="62" spans="1:1025">
+      <c r="A62" s="4">
         <v>61</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="n">
+    <row r="63" spans="1:1025">
+      <c r="A63" s="4">
         <v>62</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3" t="n">
+    <row r="64" spans="1:1025">
+      <c r="A64" s="4">
         <v>63</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3" t="n">
+    <row r="65" spans="1:1025">
+      <c r="A65" s="4">
         <v>64</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3" t="n">
+    <row r="66" spans="1:1025">
+      <c r="A66" s="4">
         <v>65</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3" t="n">
+    <row r="67" spans="1:1025">
+      <c r="A67" s="4">
         <v>66</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3" t="n">
+    <row r="68" spans="1:1025">
+      <c r="A68" s="4">
         <v>67</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="n">
+    <row r="69" spans="1:1025">
+      <c r="A69" s="4">
         <v>68</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="n">
+    <row r="70" spans="1:1025">
+      <c r="A70" s="4">
         <v>69</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="n">
+    <row r="71" spans="1:1025">
+      <c r="A71" s="4">
         <v>70</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3" t="n">
+    <row r="72" spans="1:1025">
+      <c r="A72" s="4">
         <v>71</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3" t="n">
+    <row r="73" spans="1:1025">
+      <c r="A73" s="4">
         <v>72</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3" t="n">
+    <row r="74" spans="1:1025">
+      <c r="A74" s="4">
         <v>73</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3" t="n">
+    <row r="75" spans="1:1025">
+      <c r="A75" s="4">
         <v>74</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3" t="n">
+    <row r="76" spans="1:1025">
+      <c r="A76" s="4">
         <v>75</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="n">
+    <row r="77" spans="1:1025">
+      <c r="A77" s="4">
         <v>76</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>29</v>
+      <c r="B77" s="4" t="str">
+        <v>Reserved_bank2</v>
+      </c>
+      <c r="C77" s="4" t="str">
+        <v>string3</v>
       </c>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="n">
+    <row r="78" spans="1:1025">
+      <c r="A78" s="4">
         <v>77</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3" t="n">
+    <row r="79" spans="1:1025">
+      <c r="A79" s="4">
         <v>78</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="n">
+    <row r="80" spans="1:1025">
+      <c r="A80" s="4">
         <v>79</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3" t="n">
+    <row r="81" spans="1:1025">
+      <c r="A81" s="4">
         <v>80</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="n">
+    <row r="82" spans="1:1025">
+      <c r="A82" s="4">
         <v>81</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3" t="n">
+    <row r="83" spans="1:1025">
+      <c r="A83" s="4">
         <v>82</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3" t="n">
+    <row r="84" spans="1:1025">
+      <c r="A84" s="4">
         <v>83</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="n">
+    <row r="85" spans="1:1025">
+      <c r="A85" s="4">
         <v>84</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="n">
+    <row r="86" spans="1:1025">
+      <c r="A86" s="4">
         <v>85</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="n">
+    <row r="87" spans="1:1025">
+      <c r="A87" s="4">
         <v>86</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="n">
+    <row r="88" spans="1:1025">
+      <c r="A88" s="4">
         <v>87</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="n">
+    <row r="89" spans="1:1025">
+      <c r="A89" s="4">
         <v>88</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="n">
+    <row r="90" spans="1:1025">
+      <c r="A90" s="4">
         <v>89</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="n">
+    <row r="91" spans="1:1025">
+      <c r="A91" s="4">
         <v>90</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="n">
+    <row r="92" spans="1:1025">
+      <c r="A92" s="4">
         <v>91</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="n">
+    <row r="93" spans="1:1025">
+      <c r="A93" s="4">
         <v>92</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="n">
+    <row r="94" spans="1:1025">
+      <c r="A94" s="4">
         <v>93</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="n">
+    <row r="95" spans="1:1025">
+      <c r="A95" s="4">
         <v>94</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="n">
+    <row r="96" spans="1:1025">
+      <c r="A96" s="4">
         <v>95</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="n">
+    <row r="97" spans="1:1025">
+      <c r="A97" s="4">
         <v>96</v>
       </c>
-      <c r="B97" s="4" t="s">
-        <v>30</v>
+      <c r="B97" s="4" t="str">
+        <v>Reserved_bank3</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="n">
+    <row r="98" spans="1:1025">
+      <c r="A98" s="4">
         <v>97</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="n">
+    <row r="99" spans="1:1025">
+      <c r="A99" s="4">
         <v>98</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3" t="n">
+    <row r="100" spans="1:1025">
+      <c r="A100" s="4">
         <v>99</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3" t="n">
+    <row r="101" spans="1:1025">
+      <c r="A101" s="4">
         <v>100</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3" t="n">
+    <row r="102" spans="1:1025">
+      <c r="A102" s="4">
         <v>101</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3" t="n">
+    <row r="103" spans="1:1025">
+      <c r="A103" s="4">
         <v>102</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3" t="n">
+    <row r="104" spans="1:1025">
+      <c r="A104" s="4">
         <v>103</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3" t="n">
+    <row r="105" spans="1:1025">
+      <c r="A105" s="4">
         <v>104</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="3" t="n">
+    <row r="106" spans="1:1025">
+      <c r="A106" s="4">
         <v>105</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="3" t="n">
+    <row r="107" spans="1:1025">
+      <c r="A107" s="4">
         <v>106</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="3" t="n">
+    <row r="108" spans="1:1025">
+      <c r="A108" s="4">
         <v>107</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="3" t="n">
+    <row r="109" spans="1:1025">
+      <c r="A109" s="4">
         <v>108</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="3" t="n">
+    <row r="110" spans="1:1025">
+      <c r="A110" s="4">
         <v>109</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="3" t="n">
+    <row r="111" spans="1:1025">
+      <c r="A111" s="4">
         <v>110</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="3" t="n">
+    <row r="112" spans="1:1025">
+      <c r="A112" s="4">
         <v>111</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="3" t="n">
+    <row r="113" spans="1:1025">
+      <c r="A113" s="4">
         <v>112</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="3" t="n">
+    <row r="114" spans="1:1025">
+      <c r="A114" s="4">
         <v>113</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="3" t="n">
+    <row r="115" spans="1:1025">
+      <c r="A115" s="4">
         <v>114</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="3" t="n">
+    <row r="116" spans="1:1025">
+      <c r="A116" s="4">
         <v>115</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="3" t="n">
+    <row r="117" spans="1:1025">
+      <c r="A117" s="4">
         <v>116</v>
       </c>
-      <c r="B117" s="4" t="s">
-        <v>31</v>
+      <c r="B117" s="4" t="str">
+        <v>Reserved_bank4</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="3" t="n">
+    <row r="118" spans="1:1025">
+      <c r="A118" s="4">
         <v>117</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="3" t="n">
+    <row r="119" spans="1:1025">
+      <c r="A119" s="4">
         <v>118</v>
       </c>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="3" t="n">
+    <row r="120" spans="1:1025">
+      <c r="A120" s="4">
         <v>119</v>
       </c>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="3" t="n">
+    <row r="121" spans="1:1025">
+      <c r="A121" s="4">
         <v>120</v>
       </c>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="3" t="n">
+    <row r="122" spans="1:1025">
+      <c r="A122" s="4">
         <v>121</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="3" t="n">
+    <row r="123" spans="1:1025">
+      <c r="A123" s="4">
         <v>122</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="3" t="n">
+    <row r="124" spans="1:1025">
+      <c r="A124" s="4">
         <v>123</v>
       </c>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="3" t="n">
+    <row r="125" spans="1:1025">
+      <c r="A125" s="4">
         <v>124</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="3" t="n">
+    <row r="126" spans="1:1025">
+      <c r="A126" s="4">
         <v>125</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="3" t="n">
+    <row r="127" spans="1:1025">
+      <c r="A127" s="4">
         <v>126</v>
       </c>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="3" t="n">
+    <row r="128" spans="1:1025">
+      <c r="A128" s="4">
         <v>127</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="3" t="n">
+    <row r="129" spans="1:1025">
+      <c r="A129" s="4">
         <v>128</v>
       </c>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="3" t="n">
+    <row r="130" spans="1:1025">
+      <c r="A130" s="4">
         <v>129</v>
       </c>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="3" t="n">
+    <row r="131" spans="1:1025">
+      <c r="A131" s="4">
         <v>130</v>
       </c>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="3" t="n">
+    <row r="132" spans="1:1025">
+      <c r="A132" s="4">
         <v>131</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="3" t="n">
+    <row r="133" spans="1:1025">
+      <c r="A133" s="4">
         <v>132</v>
       </c>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="3" t="n">
+    <row r="134" spans="1:1025">
+      <c r="A134" s="4">
         <v>133</v>
       </c>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="3" t="n">
+    <row r="135" spans="1:1025">
+      <c r="A135" s="4">
         <v>134</v>
       </c>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="3" t="n">
+    <row r="136" spans="1:1025">
+      <c r="A136" s="4">
         <v>135</v>
       </c>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="3" t="n">
+    <row r="137" spans="1:1025">
+      <c r="A137" s="4">
         <v>136</v>
       </c>
-      <c r="B137" s="4" t="s">
-        <v>32</v>
+      <c r="B137" s="4" t="str">
+        <v>Reserved_bank5</v>
       </c>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="3" t="n">
+    <row r="138" spans="1:1025">
+      <c r="A138" s="4">
         <v>137</v>
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="3" t="n">
+    <row r="139" spans="1:1025">
+      <c r="A139" s="4">
         <v>138</v>
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="3" t="n">
+    <row r="140" spans="1:1025">
+      <c r="A140" s="4">
         <v>139</v>
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
     </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="3" t="n">
+    <row r="141" spans="1:1025">
+      <c r="A141" s="4">
         <v>140</v>
       </c>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
     </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="3" t="n">
+    <row r="142" spans="1:1025">
+      <c r="A142" s="4">
         <v>141</v>
       </c>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
     </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="3" t="n">
+    <row r="143" spans="1:1025">
+      <c r="A143" s="4">
         <v>142</v>
       </c>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
     </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="3" t="n">
+    <row r="144" spans="1:1025">
+      <c r="A144" s="4">
         <v>143</v>
       </c>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="3" t="n">
+    <row r="145" spans="1:1025">
+      <c r="A145" s="4">
         <v>144</v>
       </c>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
     </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="3" t="n">
+    <row r="146" spans="1:1025">
+      <c r="A146" s="4">
         <v>145</v>
       </c>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
     </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="3" t="n">
+    <row r="147" spans="1:1025">
+      <c r="A147" s="4">
         <v>146</v>
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
     </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="3" t="n">
+    <row r="148" spans="1:1025">
+      <c r="A148" s="4">
         <v>147</v>
       </c>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
     </row>
-    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="3" t="n">
+    <row r="149" spans="1:1025">
+      <c r="A149" s="4">
         <v>148</v>
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="3" t="n">
+    <row r="150" spans="1:1025">
+      <c r="A150" s="4">
         <v>149</v>
       </c>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="3" t="n">
+    <row r="151" spans="1:1025">
+      <c r="A151" s="4">
         <v>150</v>
       </c>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="3" t="n">
+    <row r="152" spans="1:1025">
+      <c r="A152" s="4">
         <v>151</v>
       </c>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
     </row>
-    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="3" t="n">
+    <row r="153" spans="1:1025">
+      <c r="A153" s="4">
         <v>152</v>
       </c>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
     </row>
-    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="3" t="n">
+    <row r="154" spans="1:1025">
+      <c r="A154" s="4">
         <v>153</v>
       </c>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
     </row>
-    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="3" t="n">
+    <row r="155" spans="1:1025">
+      <c r="A155" s="4">
         <v>154</v>
       </c>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="3" t="n">
+    <row r="156" spans="1:1025">
+      <c r="A156" s="4">
         <v>155</v>
       </c>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
     </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="3" t="n">
+    <row r="157" spans="1:1025">
+      <c r="A157" s="4">
         <v>156</v>
       </c>
-      <c r="B157" s="4" t="s">
-        <v>33</v>
+      <c r="B157" s="4" t="str">
+        <v>Reserved_bank6</v>
       </c>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="3" t="n">
+    <row r="158" spans="1:1025">
+      <c r="A158" s="4">
         <v>157</v>
       </c>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="3" t="n">
+    <row r="159" spans="1:1025">
+      <c r="A159" s="4">
         <v>158</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
     </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="3" t="n">
+    <row r="160" spans="1:1025">
+      <c r="A160" s="4">
         <v>159</v>
       </c>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
     </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="3" t="n">
+    <row r="161" spans="1:1025">
+      <c r="A161" s="4">
         <v>160</v>
       </c>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
     </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="3" t="n">
+    <row r="162" spans="1:1025">
+      <c r="A162" s="4">
         <v>161</v>
       </c>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
     </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="3" t="n">
+    <row r="163" spans="1:1025">
+      <c r="A163" s="4">
         <v>162</v>
       </c>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="3" t="n">
+    <row r="164" spans="1:1025">
+      <c r="A164" s="4">
         <v>163</v>
       </c>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
     </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="3" t="n">
+    <row r="165" spans="1:1025">
+      <c r="A165" s="4">
         <v>164</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
     </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="3" t="n">
+    <row r="166" spans="1:1025">
+      <c r="A166" s="4">
         <v>165</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
     </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="3" t="n">
+    <row r="167" spans="1:1025">
+      <c r="A167" s="4">
         <v>166</v>
       </c>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
     </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="3" t="n">
+    <row r="168" spans="1:1025">
+      <c r="A168" s="4">
         <v>167</v>
       </c>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
     </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="3" t="n">
+    <row r="169" spans="1:1025">
+      <c r="A169" s="4">
         <v>168</v>
       </c>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
     </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="3" t="n">
+    <row r="170" spans="1:1025">
+      <c r="A170" s="4">
         <v>169</v>
       </c>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
     </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="3" t="n">
+    <row r="171" spans="1:1025">
+      <c r="A171" s="4">
         <v>170</v>
       </c>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
     </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="3" t="n">
+    <row r="172" spans="1:1025">
+      <c r="A172" s="4">
         <v>171</v>
       </c>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
     </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="3" t="n">
+    <row r="173" spans="1:1025">
+      <c r="A173" s="4">
         <v>172</v>
       </c>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
     </row>
-    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="3" t="n">
+    <row r="174" spans="1:1025">
+      <c r="A174" s="4">
         <v>173</v>
       </c>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="3" t="n">
+    <row r="175" spans="1:1025">
+      <c r="A175" s="4">
         <v>174</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="3" t="n">
+    <row r="176" spans="1:1025">
+      <c r="A176" s="4">
         <v>175</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="3" t="n">
+    <row r="177" spans="1:1025">
+      <c r="A177" s="4">
         <v>176</v>
       </c>
-      <c r="B177" s="4" t="s">
-        <v>34</v>
+      <c r="B177" s="4" t="str">
+        <v>Reserved_bank7</v>
       </c>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
     </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="3" t="n">
+    <row r="178" spans="1:1025">
+      <c r="A178" s="4">
         <v>177</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
     </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="3" t="n">
+    <row r="179" spans="1:1025">
+      <c r="A179" s="4">
         <v>178</v>
       </c>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
     </row>
-    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="3" t="n">
+    <row r="180" spans="1:1025">
+      <c r="A180" s="4">
         <v>179</v>
       </c>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
     </row>
-    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="3" t="n">
+    <row r="181" spans="1:1025">
+      <c r="A181" s="4">
         <v>180</v>
       </c>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
     </row>
-    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="3" t="n">
+    <row r="182" spans="1:1025">
+      <c r="A182" s="4">
         <v>181</v>
       </c>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
     </row>
-    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="3" t="n">
+    <row r="183" spans="1:1025">
+      <c r="A183" s="4">
         <v>182</v>
       </c>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
     </row>
-    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="3" t="n">
+    <row r="184" spans="1:1025">
+      <c r="A184" s="4">
         <v>183</v>
       </c>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
       <c r="D184" s="4"/>
     </row>
-    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="3" t="n">
+    <row r="185" spans="1:1025">
+      <c r="A185" s="4">
         <v>184</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
       <c r="D185" s="4"/>
     </row>
-    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="3" t="n">
+    <row r="186" spans="1:1025">
+      <c r="A186" s="4">
         <v>185</v>
       </c>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
       <c r="D186" s="4"/>
     </row>
-    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="3" t="n">
+    <row r="187" spans="1:1025">
+      <c r="A187" s="4">
         <v>186</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
       <c r="D187" s="4"/>
     </row>
-    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="3" t="n">
+    <row r="188" spans="1:1025">
+      <c r="A188" s="4">
         <v>187</v>
       </c>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
     </row>
-    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="3" t="n">
+    <row r="189" spans="1:1025">
+      <c r="A189" s="4">
         <v>188</v>
       </c>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
     </row>
-    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="3" t="n">
+    <row r="190" spans="1:1025">
+      <c r="A190" s="4">
         <v>189</v>
       </c>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
     </row>
-    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="3" t="n">
+    <row r="191" spans="1:1025">
+      <c r="A191" s="4">
         <v>190</v>
       </c>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
     </row>
-    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="3" t="n">
+    <row r="192" spans="1:1025">
+      <c r="A192" s="4">
         <v>191</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
     </row>
-    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="3" t="n">
+    <row r="193" spans="1:1025">
+      <c r="A193" s="4">
         <v>192</v>
       </c>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
       <c r="D193" s="4"/>
     </row>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="3" t="n">
+    <row r="194" spans="1:1025">
+      <c r="A194" s="4">
         <v>193</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
     </row>
-    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="3" t="n">
+    <row r="195" spans="1:1025">
+      <c r="A195" s="4">
         <v>194</v>
       </c>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
     </row>
-    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="3" t="n">
+    <row r="196" spans="1:1025">
+      <c r="A196" s="4">
         <v>195</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
     </row>
-    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="3" t="n">
+    <row r="197" spans="1:1025">
+      <c r="A197" s="4">
         <v>196</v>
       </c>
-      <c r="B197" s="4" t="s">
-        <v>35</v>
+      <c r="B197" s="4" t="str">
+        <v>reserved2</v>
       </c>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
     </row>
-    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="3" t="n">
+    <row r="198" spans="1:1025">
+      <c r="A198" s="4">
         <v>197</v>
       </c>
       <c r="B198" s="4"/>
       <c r="C198" s="4"/>
       <c r="D198" s="4"/>
     </row>
-    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="3" t="n">
+    <row r="199" spans="1:1025">
+      <c r="A199" s="4">
         <v>198</v>
       </c>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
     </row>
-    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="3" t="n">
+    <row r="200" spans="1:1025">
+      <c r="A200" s="4">
         <v>199</v>
       </c>
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
       <c r="D200" s="4"/>
     </row>
-    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="3" t="n">
+    <row r="201" spans="1:1025">
+      <c r="A201" s="4">
         <v>200</v>
       </c>
       <c r="B201" s="4"/>
       <c r="C201" s="4"/>
       <c r="D201" s="4"/>
     </row>
-    <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="3" t="n">
+    <row r="202" spans="1:1025">
+      <c r="A202" s="4">
         <v>201</v>
       </c>
       <c r="B202" s="4"/>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
     </row>
-    <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="3" t="n">
+    <row r="203" spans="1:1025">
+      <c r="A203" s="4">
         <v>202</v>
       </c>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
     </row>
-    <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="3" t="n">
+    <row r="204" spans="1:1025">
+      <c r="A204" s="4">
         <v>203</v>
       </c>
       <c r="B204" s="4"/>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
     </row>
-    <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="3" t="n">
+    <row r="205" spans="1:1025">
+      <c r="A205" s="4">
         <v>204</v>
       </c>
       <c r="B205" s="4"/>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
     </row>
-    <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="3" t="n">
+    <row r="206" spans="1:1025">
+      <c r="A206" s="4">
         <v>205</v>
       </c>
       <c r="B206" s="4"/>
       <c r="C206" s="4"/>
       <c r="D206" s="4"/>
     </row>
-    <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="3" t="n">
+    <row r="207" spans="1:1025">
+      <c r="A207" s="4">
         <v>206</v>
       </c>
       <c r="B207" s="4"/>
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
     </row>
-    <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="3" t="n">
+    <row r="208" spans="1:1025">
+      <c r="A208" s="4">
         <v>207</v>
       </c>
       <c r="B208" s="4"/>
       <c r="C208" s="4"/>
       <c r="D208" s="4"/>
     </row>
-    <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="3" t="n">
+    <row r="209" spans="1:1025">
+      <c r="A209" s="4">
         <v>208</v>
       </c>
       <c r="B209" s="4"/>
       <c r="C209" s="4"/>
       <c r="D209" s="4"/>
     </row>
-    <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="3" t="n">
+    <row r="210" spans="1:1025">
+      <c r="A210" s="4">
         <v>209</v>
       </c>
       <c r="B210" s="4"/>
       <c r="C210" s="4"/>
       <c r="D210" s="4"/>
     </row>
-    <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="3" t="n">
+    <row r="211" spans="1:1025">
+      <c r="A211" s="4">
         <v>210</v>
       </c>
       <c r="B211" s="4"/>
       <c r="C211" s="4"/>
       <c r="D211" s="4"/>
     </row>
-    <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="3" t="n">
+    <row r="212" spans="1:1025">
+      <c r="A212" s="4">
         <v>211</v>
       </c>
       <c r="B212" s="4"/>
       <c r="C212" s="4"/>
       <c r="D212" s="4"/>
     </row>
-    <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="3" t="n">
+    <row r="213" spans="1:1025">
+      <c r="A213" s="4">
         <v>212</v>
       </c>
       <c r="B213" s="4"/>
       <c r="C213" s="4"/>
       <c r="D213" s="4"/>
     </row>
-    <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="3" t="n">
+    <row r="214" spans="1:1025">
+      <c r="A214" s="4">
         <v>213</v>
       </c>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
     </row>
-    <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="3" t="n">
+    <row r="215" spans="1:1025">
+      <c r="A215" s="4">
         <v>214</v>
       </c>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
     </row>
-    <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="3" t="n">
+    <row r="216" spans="1:1025">
+      <c r="A216" s="4">
         <v>215</v>
       </c>
       <c r="B216" s="4"/>
       <c r="C216" s="4"/>
       <c r="D216" s="4"/>
     </row>
-    <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="3" t="n">
+    <row r="217" spans="1:1025">
+      <c r="A217" s="4">
         <v>216</v>
       </c>
       <c r="B217" s="4"/>
       <c r="C217" s="4"/>
       <c r="D217" s="4"/>
     </row>
-    <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="3" t="n">
+    <row r="218" spans="1:1025">
+      <c r="A218" s="4">
         <v>217</v>
       </c>
       <c r="B218" s="4"/>
       <c r="C218" s="4"/>
       <c r="D218" s="4"/>
     </row>
-    <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="3" t="n">
+    <row r="219" spans="1:1025">
+      <c r="A219" s="4">
         <v>218</v>
       </c>
       <c r="B219" s="4"/>
       <c r="C219" s="4"/>
       <c r="D219" s="4"/>
     </row>
-    <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="3" t="n">
+    <row r="220" spans="1:1025">
+      <c r="A220" s="4">
         <v>219</v>
       </c>
       <c r="B220" s="4"/>
       <c r="C220" s="4"/>
       <c r="D220" s="4"/>
     </row>
-    <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="3" t="n">
+    <row r="221" spans="1:1025">
+      <c r="A221" s="4">
         <v>220</v>
       </c>
       <c r="B221" s="4"/>
       <c r="C221" s="4"/>
       <c r="D221" s="4"/>
     </row>
-    <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="3" t="n">
+    <row r="222" spans="1:1025">
+      <c r="A222" s="4">
         <v>221</v>
       </c>
       <c r="B222" s="4"/>
       <c r="C222" s="4"/>
       <c r="D222" s="4"/>
     </row>
-    <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="3" t="n">
+    <row r="223" spans="1:1025">
+      <c r="A223" s="4">
         <v>222</v>
       </c>
       <c r="B223" s="4"/>
       <c r="C223" s="4"/>
       <c r="D223" s="4"/>
     </row>
-    <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="3" t="n">
+    <row r="224" spans="1:1025">
+      <c r="A224" s="4">
         <v>223</v>
       </c>
       <c r="B224" s="4"/>
       <c r="C224" s="4"/>
       <c r="D224" s="4"/>
     </row>
-    <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="3" t="n">
+    <row r="225" spans="1:1025">
+      <c r="A225" s="4">
         <v>224</v>
       </c>
       <c r="B225" s="4"/>
       <c r="C225" s="4"/>
       <c r="D225" s="4"/>
     </row>
-    <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="3" t="n">
+    <row r="226" spans="1:1025">
+      <c r="A226" s="4">
         <v>225</v>
       </c>
       <c r="B226" s="4"/>
       <c r="C226" s="4"/>
       <c r="D226" s="4"/>
     </row>
-    <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="3" t="n">
+    <row r="227" spans="1:1025">
+      <c r="A227" s="4">
         <v>226</v>
       </c>
       <c r="B227" s="4"/>
       <c r="C227" s="4"/>
       <c r="D227" s="4"/>
     </row>
-    <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="3" t="n">
+    <row r="228" spans="1:1025">
+      <c r="A228" s="4">
         <v>227</v>
       </c>
       <c r="B228" s="4"/>
       <c r="C228" s="4"/>
       <c r="D228" s="4"/>
     </row>
-    <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="3" t="n">
+    <row r="229" spans="1:1025">
+      <c r="A229" s="4">
         <v>228</v>
       </c>
       <c r="B229" s="4"/>
       <c r="C229" s="4"/>
       <c r="D229" s="4"/>
     </row>
-    <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="3" t="n">
+    <row r="230" spans="1:1025">
+      <c r="A230" s="4">
         <v>229</v>
       </c>
       <c r="B230" s="4"/>
       <c r="C230" s="4"/>
       <c r="D230" s="4"/>
     </row>
-    <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="3" t="n">
+    <row r="231" spans="1:1025">
+      <c r="A231" s="4">
         <v>230</v>
       </c>
       <c r="B231" s="4"/>
       <c r="C231" s="4"/>
       <c r="D231" s="4"/>
     </row>
-    <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="3" t="n">
+    <row r="232" spans="1:1025">
+      <c r="A232" s="4">
         <v>231</v>
       </c>
       <c r="B232" s="4"/>
       <c r="C232" s="4"/>
       <c r="D232" s="4"/>
     </row>
-    <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="3" t="n">
+    <row r="233" spans="1:1025">
+      <c r="A233" s="4">
         <v>232</v>
       </c>
       <c r="B233" s="4"/>
       <c r="C233" s="4"/>
       <c r="D233" s="4"/>
     </row>
-    <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="3" t="n">
+    <row r="234" spans="1:1025">
+      <c r="A234" s="4">
         <v>233</v>
       </c>
       <c r="B234" s="4"/>
       <c r="C234" s="4"/>
       <c r="D234" s="4"/>
     </row>
-    <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="3" t="n">
+    <row r="235" spans="1:1025">
+      <c r="A235" s="4">
         <v>234</v>
       </c>
       <c r="B235" s="4"/>
       <c r="C235" s="4"/>
       <c r="D235" s="4"/>
     </row>
-    <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="3" t="n">
+    <row r="236" spans="1:1025">
+      <c r="A236" s="4">
         <v>235</v>
       </c>
       <c r="B236" s="4"/>
       <c r="C236" s="4"/>
       <c r="D236" s="4"/>
     </row>
-    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="3" t="n">
+    <row r="237" spans="1:1025">
+      <c r="A237" s="4">
         <v>236</v>
       </c>
       <c r="B237" s="4"/>
       <c r="C237" s="4"/>
       <c r="D237" s="4"/>
     </row>
-    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="3" t="n">
+    <row r="238" spans="1:1025">
+      <c r="A238" s="4">
         <v>237</v>
       </c>
       <c r="B238" s="4"/>
       <c r="C238" s="4"/>
       <c r="D238" s="4"/>
     </row>
-    <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="3" t="n">
+    <row r="239" spans="1:1025">
+      <c r="A239" s="4">
         <v>238</v>
       </c>
       <c r="B239" s="4"/>
       <c r="C239" s="4"/>
       <c r="D239" s="4"/>
     </row>
-    <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="3" t="n">
+    <row r="240" spans="1:1025">
+      <c r="A240" s="4">
         <v>239</v>
       </c>
-      <c r="B240" s="3" t="s">
-        <v>36</v>
+      <c r="B240" s="4" t="str">
+        <v>Enable Network?</v>
       </c>
       <c r="C240" s="4"/>
       <c r="D240" s="4"/>
     </row>
-    <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="3" t="n">
+    <row r="241" spans="1:1025">
+      <c r="A241" s="4">
         <v>240</v>
       </c>
-      <c r="B241" s="3" t="s">
-        <v>37</v>
+      <c r="B241" s="4" t="str">
+        <v>Use DHCP?</v>
       </c>
       <c r="C241" s="4"/>
       <c r="D241" s="4"/>
     </row>
-    <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="3" t="n">
+    <row r="242" spans="1:1025">
+      <c r="A242" s="4">
         <v>241</v>
       </c>
-      <c r="B242" s="4" t="s">
-        <v>38</v>
+      <c r="B242" s="4" t="str">
+        <v>IP address</v>
       </c>
       <c r="C242" s="4"/>
       <c r="D242" s="4"/>
     </row>
-    <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="3" t="n">
+    <row r="243" spans="1:1025">
+      <c r="A243" s="4">
         <v>242</v>
       </c>
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
       <c r="D243" s="4"/>
     </row>
-    <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="3" t="n">
+    <row r="244" spans="1:1025">
+      <c r="A244" s="4">
         <v>243</v>
       </c>
       <c r="B244" s="4"/>
       <c r="C244" s="4"/>
       <c r="D244" s="4"/>
     </row>
-    <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="3" t="n">
+    <row r="245" spans="1:1025">
+      <c r="A245" s="4">
         <v>244</v>
       </c>
       <c r="B245" s="4"/>
       <c r="C245" s="4"/>
       <c r="D245" s="4"/>
     </row>
-    <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="3" t="n">
+    <row r="246" spans="1:1025">
+      <c r="A246" s="4">
         <v>245</v>
       </c>
-      <c r="B246" s="4" t="s">
-        <v>39</v>
+      <c r="B246" s="4" t="str">
+        <v>Gateway</v>
       </c>
       <c r="C246" s="4"/>
       <c r="D246" s="4"/>
     </row>
-    <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="3" t="n">
+    <row r="247" spans="1:1025">
+      <c r="A247" s="4">
         <v>246</v>
       </c>
       <c r="B247" s="4"/>
       <c r="C247" s="4"/>
       <c r="D247" s="4"/>
     </row>
-    <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="3" t="n">
+    <row r="248" spans="1:1025">
+      <c r="A248" s="4">
         <v>247</v>
       </c>
       <c r="B248" s="4"/>
       <c r="C248" s="4"/>
       <c r="D248" s="4"/>
     </row>
-    <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="3" t="n">
+    <row r="249" spans="1:1025">
+      <c r="A249" s="4">
         <v>248</v>
       </c>
       <c r="B249" s="4"/>
       <c r="C249" s="4"/>
       <c r="D249" s="4"/>
     </row>
-    <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="3" t="n">
+    <row r="250" spans="1:1025">
+      <c r="A250" s="4">
         <v>249</v>
       </c>
-      <c r="B250" s="4" t="s">
-        <v>40</v>
+      <c r="B250" s="4" t="str">
+        <v>DNS1</v>
       </c>
       <c r="C250" s="4"/>
       <c r="D250" s="4"/>
     </row>
-    <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="3" t="n">
+    <row r="251" spans="1:1025">
+      <c r="A251" s="4">
         <v>250</v>
       </c>
       <c r="B251" s="4"/>
       <c r="C251" s="4"/>
       <c r="D251" s="4"/>
     </row>
-    <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="3" t="n">
+    <row r="252" spans="1:1025">
+      <c r="A252" s="4">
         <v>251</v>
       </c>
       <c r="B252" s="4"/>
       <c r="C252" s="4"/>
       <c r="D252" s="4"/>
     </row>
-    <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="3" t="n">
+    <row r="253" spans="1:1025">
+      <c r="A253" s="4">
         <v>252</v>
       </c>
       <c r="B253" s="4"/>
       <c r="C253" s="4"/>
       <c r="D253" s="4"/>
     </row>
-    <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="3" t="n">
+    <row r="254" spans="1:1025">
+      <c r="A254" s="4">
         <v>253</v>
       </c>
-      <c r="B254" s="4" t="s">
-        <v>41</v>
+      <c r="B254" s="4" t="str">
+        <v>DNS2</v>
       </c>
       <c r="C254" s="4"/>
       <c r="D254" s="4"/>
     </row>
-    <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="3" t="n">
+    <row r="255" spans="1:1025">
+      <c r="A255" s="4">
         <v>254</v>
       </c>
       <c r="B255" s="4"/>
       <c r="C255" s="4"/>
       <c r="D255" s="4"/>
     </row>
-    <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="3" t="n">
+    <row r="256" spans="1:1025">
+      <c r="A256" s="4">
         <v>255</v>
       </c>
       <c r="B256" s="4"/>
       <c r="C256" s="4"/>
       <c r="D256" s="4"/>
     </row>
-    <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="3" t="n">
+    <row r="257" spans="1:1025">
+      <c r="A257" s="4">
         <v>256</v>
       </c>
       <c r="B257" s="4"/>
@@ -2444,90 +2335,83 @@
       <c r="D257" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="D2:D257"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="C17:C36"/>
-    <mergeCell ref="B23:B36"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <mergeCells>
+    <mergeCell ref="B254:B257"/>
+    <mergeCell ref="B250:B253"/>
+    <mergeCell ref="B246:B249"/>
+    <mergeCell ref="B242:B245"/>
+    <mergeCell ref="B197:B239"/>
+    <mergeCell ref="B177:B196"/>
+    <mergeCell ref="B157:B176"/>
+    <mergeCell ref="B137:B156"/>
+    <mergeCell ref="B117:B136"/>
+    <mergeCell ref="B97:B116"/>
+    <mergeCell ref="C97:C257"/>
+    <mergeCell ref="B77:B96"/>
+    <mergeCell ref="C77:C96"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="C57:C76"/>
     <mergeCell ref="B37:B56"/>
     <mergeCell ref="C37:C56"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="C57:C76"/>
-    <mergeCell ref="B77:B96"/>
-    <mergeCell ref="C77:C96"/>
-    <mergeCell ref="B97:B116"/>
-    <mergeCell ref="C97:C257"/>
-    <mergeCell ref="B117:B136"/>
-    <mergeCell ref="B137:B156"/>
-    <mergeCell ref="B157:B176"/>
-    <mergeCell ref="B177:B196"/>
-    <mergeCell ref="B197:B239"/>
-    <mergeCell ref="B242:B245"/>
-    <mergeCell ref="B246:B249"/>
-    <mergeCell ref="B250:B253"/>
-    <mergeCell ref="B254:B257"/>
+    <mergeCell ref="B25:B36"/>
+    <mergeCell ref="C17:C36"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="D2:D257"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.5118" footer="0.5118"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" fitToHeight="1" fitToWidth="1" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
     <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AMK1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5748987854251"/>
+    <col min="1" max="1025" style="7" width="10.5749" bestFit="1" customWidth="1"/>
+    <col min="1026" max="16384" style="7"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.5118" footer="0.5118"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" fitToHeight="1" fitToWidth="1" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
     <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AMK1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5748987854251"/>
+    <col min="1" max="1025" style="8" width="10.5749" bestFit="1" customWidth="1"/>
+    <col min="1026" max="16384" style="8"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.5118" footer="0.5118"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" fitToHeight="1" fitToWidth="1" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
 </worksheet>
 </file>
</xml_diff>